<commit_message>
auto commit by win-upload.bat
</commit_message>
<xml_diff>
--- a/Verification-GraphMaking/DataManipulation/confidence_interval.xlsx
+++ b/Verification-GraphMaking/DataManipulation/confidence_interval.xlsx
@@ -423,10 +423,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.008391601735757488</v>
+        <v>0.008391601385890152</v>
       </c>
       <c r="B1" t="n">
-        <v>0.04872867526177629</v>
+        <v>0.04872867561169195</v>
       </c>
       <c r="C1" t="n">
         <v>-0.072238</v>
@@ -437,10 +437,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.0116141108575662</v>
+        <v>0.01161411038278952</v>
       </c>
       <c r="B2" t="n">
-        <v>0.03894013437203862</v>
+        <v>0.0389401348469028</v>
       </c>
       <c r="C2" t="n">
         <v>-0.07527400000000001</v>
@@ -451,10 +451,10 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.01153192337079392</v>
+        <v>0.01153192313451969</v>
       </c>
       <c r="B3" t="n">
-        <v>0.03922965157552526</v>
+        <v>0.03922965181181994</v>
       </c>
       <c r="C3" t="n">
         <v>-0.075308</v>
@@ -465,10 +465,10 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.008838327130064209</v>
+        <v>0.008838327026003262</v>
       </c>
       <c r="B4" t="n">
-        <v>0.06518827903259505</v>
+        <v>0.06518827913666908</v>
       </c>
       <c r="C4" t="n">
         <v>-0.063307</v>
@@ -479,10 +479,10 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.008317400780233058</v>
+        <v>0.008317400607029065</v>
       </c>
       <c r="B5" t="n">
-        <v>0.06287601531427391</v>
+        <v>0.06287601548751062</v>
       </c>
       <c r="C5" t="n">
         <v>-0.064385</v>
@@ -493,10 +493,10 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.001533073090420826</v>
+        <v>0.001533072903790681</v>
       </c>
       <c r="B6" t="n">
-        <v>0.03496122384980356</v>
+        <v>0.03496122403647874</v>
       </c>
       <c r="C6" t="n">
         <v>-0.06986299999999999</v>
@@ -507,10 +507,10 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.01817094646073859</v>
+        <v>0.01817094582684237</v>
       </c>
       <c r="B7" t="n">
-        <v>0.04259654677834398</v>
+        <v>0.04259654741230261</v>
       </c>
       <c r="C7" t="n">
         <v>-0.05930700000000001</v>
@@ -521,10 +521,10 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.02830246822834591</v>
+        <v>0.02830246757163751</v>
       </c>
       <c r="B8" t="n">
-        <v>0.05100917381994471</v>
+        <v>0.05100917447664807</v>
       </c>
       <c r="C8" t="n">
         <v>-0.04722700000000001</v>
@@ -535,10 +535,10 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.0152292321462264</v>
+        <v>0.01522923192528239</v>
       </c>
       <c r="B9" t="n">
-        <v>0.04168562344092248</v>
+        <v>0.04168562366187897</v>
       </c>
       <c r="C9" t="n">
         <v>-0.061337</v>
@@ -549,10 +549,10 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.02355238403841944</v>
+        <v>0.02355238356857322</v>
       </c>
       <c r="B10" t="n">
-        <v>0.05612153853121771</v>
+        <v>0.056121539001087</v>
       </c>
       <c r="C10" t="n">
         <v>-0.05055900000000001</v>

</xml_diff>